<commit_message>
Working on Execution by Rows
</commit_message>
<xml_diff>
--- a/Framework/styxframework/src/main/java/excelOps/Styx.xlsx
+++ b/Framework/styxframework/src/main/java/excelOps/Styx.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8565" activeTab="1" xr2:uid="{A0608B55-7DFE-418F-9C5B-8C7B58572C7E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8565" xr2:uid="{A0608B55-7DFE-418F-9C5B-8C7B58572C7E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
+    <sheet name="Test_Cases" sheetId="2" r:id="rId1"/>
     <sheet name="Data" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
@@ -414,7 +414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08ED6BFC-0FA6-47AC-849F-C86612FC870D}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -461,7 +461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5631238B-ED84-4DD9-8F6F-86DC17F9D8D2}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>